<commit_message>
Updates to attributes fill after import
</commit_message>
<xml_diff>
--- a/PRODUCT ATTRIBUTES.xlsx
+++ b/PRODUCT ATTRIBUTES.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1088eec3f04f0d1/Documents/IFM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="188" documentId="8_{3BD5F4D7-065C-4DBA-968F-376513DE6343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D705D1E-60C8-4AF5-9876-C2F1811C65F7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EE27FD4-69EA-494E-99C6-7B6DF0512371}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{75C1FF69-647E-4D64-B2BB-F7843AAFD322}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="57">
   <si>
     <t>Type</t>
   </si>
@@ -189,6 +189,24 @@
   </si>
   <si>
     <t>ManufacturerName</t>
+  </si>
+  <si>
+    <t>Batteries</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>AMP hr</t>
+  </si>
+  <si>
+    <t>CCA</t>
+  </si>
+  <si>
+    <t>Thread Type</t>
+  </si>
+  <si>
+    <t>psi</t>
   </si>
 </sst>
 </file>
@@ -256,6 +274,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -575,13 +597,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D42C803-F4B7-4147-A731-8F8A7D2A692B}">
-  <dimension ref="A2:Q18"/>
+  <dimension ref="A2:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="3" topLeftCell="J4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +624,7 @@
     <col min="17" max="17" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -622,7 +644,7 @@
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>42</v>
       </c>
@@ -671,8 +693,11 @@
       <c r="Q3" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>30</v>
       </c>
@@ -716,7 +741,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -733,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
@@ -770,8 +795,11 @@
       <c r="Q6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
@@ -805,8 +833,11 @@
       <c r="Q7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
@@ -822,11 +853,17 @@
       <c r="L8" t="s">
         <v>20</v>
       </c>
+      <c r="M8" t="s">
+        <v>56</v>
+      </c>
       <c r="N8" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
@@ -840,7 +877,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -854,7 +891,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
@@ -883,7 +920,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
@@ -897,7 +934,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>50</v>
       </c>
@@ -920,7 +957,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -937,12 +974,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C15" t="s">
         <v>39</v>
+      </c>
+      <c r="G15" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" t="s">
+        <v>55</v>
       </c>
       <c r="N15" t="s">
         <v>17</v>

</xml_diff>